<commit_message>
IndMF- Added 52 week data
</commit_message>
<xml_diff>
--- a/Reports/IndMFData/IndMF_SmallCap.xlsx
+++ b/Reports/IndMFData/IndMF_SmallCap.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i852841/_Codes/_Personal/StockRankingCrawler/Reports/IndMFData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869D588C-E8F5-D244-B7C1-AF5BF41DEDB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{4E0B69B5-FFEB-C54D-8763-8253AD0074FA}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="7" windowHeight="19380" windowWidth="33600" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="460"/>
   </bookViews>
   <sheets>
-    <sheet name="SmallCap" sheetId="1" r:id="rId1"/>
-    <sheet name="UNDERLYINGINDEX" sheetId="2" r:id="rId2"/>
-    <sheet name="AUM" sheetId="3" r:id="rId3"/>
-    <sheet name="EXPENSERATIO" sheetId="4" r:id="rId4"/>
-    <sheet name="MANAGER" sheetId="5" r:id="rId5"/>
-    <sheet name="PERATIO" sheetId="6" r:id="rId6"/>
-    <sheet name="PBRATIO" sheetId="7" r:id="rId7"/>
+    <sheet name="SmallCap" r:id="rId1" sheetId="1"/>
+    <sheet name="UNDERLYINGINDEX" r:id="rId2" sheetId="2"/>
+    <sheet name="AUM" r:id="rId3" sheetId="3"/>
+    <sheet name="EXPENSERATIO" r:id="rId4" sheetId="4"/>
+    <sheet name="MANAGER" r:id="rId5" sheetId="5"/>
+    <sheet name="PERATIO" r:id="rId6" sheetId="6"/>
+    <sheet name="PBRATIO" r:id="rId7" sheetId="7"/>
+    <sheet name="52Week" r:id="rId8" sheetId="8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="162">
   <si>
     <t>Nov_21</t>
   </si>
@@ -449,12 +450,96 @@
   </si>
   <si>
     <t>1.79%</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>39.30 --- 47.98 
+ 22-Aug-2019 --- 02-Apr-2019</t>
+  </si>
+  <si>
+    <t>26.86 --- 33.98 
+ 10-Dec-2018 --- 04-Nov-2019</t>
+  </si>
+  <si>
+    <t>49.72 --- 58.52 
+ 18-Feb-2019 --- 04-Nov-2019</t>
+  </si>
+  <si>
+    <t>67.92 --- 78.70 
+ 05-Aug-2019 --- 03-Jun-2019</t>
+  </si>
+  <si>
+    <t>36.21 --- 43.87 
+ 22-Aug-2019 --- 27-May-2019</t>
+  </si>
+  <si>
+    <t>49.61 --- 59.25 
+ 22-Aug-2019 --- 28-May-2019</t>
+  </si>
+  <si>
+    <t>22.17 --- 27.42 
+ 18-Feb-2019 --- 04-Jun-2019</t>
+  </si>
+  <si>
+    <t>9.57 --- 10.92 
+ 05-Aug-2019 --- 27-May-2019</t>
+  </si>
+  <si>
+    <t>30.03 --- 38.16 
+ 23-Aug-2019 --- 01-Apr-2019</t>
+  </si>
+  <si>
+    <t>9.96 --- 10.72 
+ 07-Oct-2019 --- 04-Nov-2019</t>
+  </si>
+  <si>
+    <t>8.58 --- 10.15 
+ 22-Aug-2019 --- 28-May-2019</t>
+  </si>
+  <si>
+    <t>70.67 --- 88.90 
+ 22-Aug-2019 --- 28-May-2019</t>
+  </si>
+  <si>
+    <t>9.36 --- 10.91 
+ 22-Aug-2019 --- 28-May-2019</t>
+  </si>
+  <si>
+    <t>9.85 --- 11.57 
+ 05-Aug-2019 --- 28-May-2019</t>
+  </si>
+  <si>
+    <t>49.44 --- 59.27 
+ 22-Aug-2019 --- 01-Apr-2019</t>
+  </si>
+  <si>
+    <t>8.61 --- 10.59 
+ 23-Aug-2019 --- 15-Apr-2019</t>
+  </si>
+  <si>
+    <t>43.63 --- 53.34 
+ 22-Aug-2019 --- 02-Apr-2019</t>
+  </si>
+  <si>
+    <t>9.11 --- 10.31 
+ 22-Aug-2019 --- 28-May-2019</t>
+  </si>
+  <si>
+    <t>36.46 --- 53.78 
+ 22-Aug-2019 --- 19-Dec-2018</t>
+  </si>
+  <si>
+    <t>12.45 --- 14.71 
+ 22-Aug-2019 --- 16-Apr-2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -492,256 +577,278 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="269">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="291">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="10" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -766,10 +873,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -786,10 +893,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -824,7 +931,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -876,7 +983,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -987,21 +1094,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1018,7 +1125,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1070,26 +1177,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.1640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.1640625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.83203125" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="8.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1454,12 +1560,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E10517-3041-A548-8327-A322F0969D22}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E10517-3041-A548-8327-A322F0969D22}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1468,9 +1574,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="13.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="25.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1724,12 +1830,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31A2CC3-117B-3044-9A40-45E232EE90D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31A2CC3-117B-3044-9A40-45E232EE90D3}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1738,9 +1844,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="13.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="10.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1994,12 +2100,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7F83E3-8D7E-E84F-B4A5-9AABCBB25C75}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7F83E3-8D7E-E84F-B4A5-9AABCBB25C75}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2008,9 +2114,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="13.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="7.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="7.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2264,12 +2370,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1FCE02-3D0C-1545-8192-6E055D0C99D5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1FCE02-3D0C-1545-8192-6E055D0C99D5}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2278,9 +2384,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="13.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="19.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2534,12 +2640,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6044C64-1C8D-2144-BC85-693CF5996D95}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6044C64-1C8D-2144-BC85-693CF5996D95}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2548,9 +2654,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="13.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="11.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2804,12 +2910,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311CB058-A4EB-6F43-B724-C153741DCABC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311CB058-A4EB-6F43-B724-C153741DCABC}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2818,9 +2924,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="13.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="9.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -3074,6 +3180,276 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E466B42B-1FD8-C746-8F67-0DBD703B7828}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.0" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="268"/>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="268" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="268" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="269" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="268" t="n">
+        <v>41.023</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="268" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="270" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="268" t="n">
+        <v>23.527</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="268" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="271" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="268" t="n">
+        <v>33.54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="268" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="272" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="268" t="n">
+        <v>58.0555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="268" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="273" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="268" t="n">
+        <v>77.439</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="268" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="274" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="268" t="n">
+        <v>40.7476</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="268" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="275" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="268" t="n">
+        <v>54.134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="268" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="276" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" s="268" t="n">
+        <v>26.14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="268" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="277" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="268" t="n">
+        <v>10.7489</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="268" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="278" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" s="268" t="n">
+        <v>32.2205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="268" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="279" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="268" t="n">
+        <v>10.5183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="268" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="280" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" s="268" t="n">
+        <v>9.42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="268" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="281" t="s">
+        <v>153</v>
+      </c>
+      <c r="C14" s="268" t="n">
+        <v>78.0468</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="268" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="282" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15" s="268" t="n">
+        <v>10.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="268" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="283" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" s="268" t="n">
+        <v>10.945</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="268" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="284" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" s="268" t="n">
+        <v>52.7536</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="268" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="285" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="268" t="n">
+        <v>10.38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="268" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="286" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="268" t="n">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="268" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="287" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="268" t="n">
+        <v>45.3514</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="268" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="288" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" s="268" t="n">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="268" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="289" t="s">
+        <v>160</v>
+      </c>
+      <c r="C22" s="268" t="n">
+        <v>41.3028</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="268" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="290" t="s">
+        <v>161</v>
+      </c>
+      <c r="C23" s="268" t="n">
+        <v>14.44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IndMF- Added 52 week data with current NAV
</commit_message>
<xml_diff>
--- a/Reports/IndMFData/IndMF_SmallCap.xlsx
+++ b/Reports/IndMFData/IndMF_SmallCap.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i852841/_Codes/_Personal/StockRankingCrawler/Reports/IndMFData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{4E0B69B5-FFEB-C54D-8763-8253AD0074FA}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BD4573-9AEC-8243-9C40-D4EE0E198C73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="7" windowHeight="19380" windowWidth="33600" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SmallCap" r:id="rId1" sheetId="1"/>
-    <sheet name="UNDERLYINGINDEX" r:id="rId2" sheetId="2"/>
-    <sheet name="AUM" r:id="rId3" sheetId="3"/>
-    <sheet name="EXPENSERATIO" r:id="rId4" sheetId="4"/>
-    <sheet name="MANAGER" r:id="rId5" sheetId="5"/>
-    <sheet name="PERATIO" r:id="rId6" sheetId="6"/>
-    <sheet name="PBRATIO" r:id="rId7" sheetId="7"/>
-    <sheet name="52Week" r:id="rId8" sheetId="8"/>
+    <sheet name="SmallCap" sheetId="1" r:id="rId1"/>
+    <sheet name="UNDERLYINGINDEX" sheetId="2" r:id="rId2"/>
+    <sheet name="AUM" sheetId="3" r:id="rId3"/>
+    <sheet name="EXPENSERATIO" sheetId="4" r:id="rId4"/>
+    <sheet name="MANAGER" sheetId="5" r:id="rId5"/>
+    <sheet name="PERATIO" sheetId="6" r:id="rId6"/>
+    <sheet name="PBRATIO" sheetId="7" r:id="rId7"/>
+    <sheet name="52Week" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="181">
   <si>
     <t>Nov_21</t>
   </si>
@@ -450,9 +450,6 @@
   </si>
   <si>
     <t>1.79%</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>39.30 --- 47.98 
@@ -532,6 +529,86 @@
   </si>
   <si>
     <t>12.45 --- 14.71 
+ 22-Aug-2019 --- 16-Apr-2019</t>
+  </si>
+  <si>
+    <t>₹41.02 ::: 39.30 --- 47.98 
+ 22-Aug-2019 --- 02-Apr-2019</t>
+  </si>
+  <si>
+    <t>₹33.54 ::: 26.86 --- 33.98 
+ 10-Dec-2018 --- 04-Nov-2019</t>
+  </si>
+  <si>
+    <t>₹58.06 ::: 49.72 --- 58.52 
+ 18-Feb-2019 --- 04-Nov-2019</t>
+  </si>
+  <si>
+    <t>₹77.44 ::: 67.92 --- 78.70 
+ 05-Aug-2019 --- 03-Jun-2019</t>
+  </si>
+  <si>
+    <t>₹40.75 ::: 36.21 --- 43.87 
+ 22-Aug-2019 --- 27-May-2019</t>
+  </si>
+  <si>
+    <t>₹54.13 ::: 49.61 --- 59.25 
+ 22-Aug-2019 --- 28-May-2019</t>
+  </si>
+  <si>
+    <t>₹26.14 ::: 22.17 --- 27.42 
+ 18-Feb-2019 --- 04-Jun-2019</t>
+  </si>
+  <si>
+    <t>₹10.75 ::: 9.57 --- 10.92 
+ 05-Aug-2019 --- 27-May-2019</t>
+  </si>
+  <si>
+    <t>₹32.22 ::: 30.03 --- 38.16 
+ 23-Aug-2019 --- 01-Apr-2019</t>
+  </si>
+  <si>
+    <t>₹10.52 ::: 9.96 --- 10.72 
+ 07-Oct-2019 --- 04-Nov-2019</t>
+  </si>
+  <si>
+    <t>₹9.42 ::: 8.58 --- 10.15 
+ 22-Aug-2019 --- 28-May-2019</t>
+  </si>
+  <si>
+    <t>₹78.05 ::: 70.67 --- 88.90 
+ 22-Aug-2019 --- 28-May-2019</t>
+  </si>
+  <si>
+    <t>₹10.75 ::: 9.36 --- 10.91 
+ 22-Aug-2019 --- 28-May-2019</t>
+  </si>
+  <si>
+    <t>₹10.94 ::: 9.85 --- 11.57 
+ 05-Aug-2019 --- 28-May-2019</t>
+  </si>
+  <si>
+    <t>₹52.75 ::: 49.44 --- 59.27 
+ 22-Aug-2019 --- 01-Apr-2019</t>
+  </si>
+  <si>
+    <t>₹9.5 ::: 8.61 --- 10.59 
+ 23-Aug-2019 --- 15-Apr-2019</t>
+  </si>
+  <si>
+    <t>₹45.35 ::: 43.63 --- 53.34 
+ 22-Aug-2019 --- 02-Apr-2019</t>
+  </si>
+  <si>
+    <t>₹10.25 ::: 9.11 --- 10.31 
+ 22-Aug-2019 --- 28-May-2019</t>
+  </si>
+  <si>
+    <t>₹41.30 ::: 36.46 --- 53.78 
+ 22-Aug-2019 --- 19-Dec-2018</t>
+  </si>
+  <si>
+    <t>₹14.44 ::: 12.45 --- 14.71 
  22-Aug-2019 --- 16-Apr-2019</t>
   </si>
 </sst>
@@ -539,7 +616,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -577,278 +653,300 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="291">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="10" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="313">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -873,10 +971,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -893,10 +991,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -931,7 +1029,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -983,7 +1081,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1094,21 +1192,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1125,7 +1223,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1177,14 +1275,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1193,9 +1291,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.83203125" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="8.1640625" collapsed="true"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="8.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1560,12 +1658,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E10517-3041-A548-8327-A322F0969D22}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E10517-3041-A548-8327-A322F0969D22}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1574,9 +1672,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="13.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="25.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.33203125" collapsed="true"/>
+    <col min="1" max="1" width="13.83203125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1830,12 +1928,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31A2CC3-117B-3044-9A40-45E232EE90D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31A2CC3-117B-3044-9A40-45E232EE90D3}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1844,9 +1942,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="13.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="10.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="1" max="1" width="13.83203125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2100,12 +2198,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7F83E3-8D7E-E84F-B4A5-9AABCBB25C75}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7F83E3-8D7E-E84F-B4A5-9AABCBB25C75}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2114,9 +2212,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="13.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="7.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="1" max="1" width="13.83203125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2370,12 +2468,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1FCE02-3D0C-1545-8192-6E055D0C99D5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1FCE02-3D0C-1545-8192-6E055D0C99D5}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2384,9 +2482,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="13.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="19.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.5" collapsed="true"/>
+    <col min="1" max="1" width="13.83203125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2640,12 +2738,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6044C64-1C8D-2144-BC85-693CF5996D95}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6044C64-1C8D-2144-BC85-693CF5996D95}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2654,9 +2752,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="13.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="11.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="1" max="1" width="13.83203125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2910,12 +3008,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311CB058-A4EB-6F43-B724-C153741DCABC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311CB058-A4EB-6F43-B724-C153741DCABC}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2924,9 +3022,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="13.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="9.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="1" max="1" width="13.83203125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -3180,276 +3278,276 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E466B42B-1FD8-C746-8F67-0DBD703B7828}">
-  <dimension ref="A1:B23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E466B42B-1FD8-C746-8F67-0DBD703B7828}">
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.0" collapsed="false"/>
+    <col min="2" max="2" width="43.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="268"/>
       <c r="B1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="268" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="268" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="269" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="268" t="n">
-        <v>41.023</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="291" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="269" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="268" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="270" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" s="268" t="n">
-        <v>23.527</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="292" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="270" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="268" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="271" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" s="268" t="n">
-        <v>33.54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="293" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="271" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="268" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="272" t="s">
-        <v>144</v>
-      </c>
-      <c r="C5" s="268" t="n">
-        <v>58.0555</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="294" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="272" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="268" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="273" t="s">
-        <v>145</v>
-      </c>
-      <c r="C6" s="268" t="n">
-        <v>77.439</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="295" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="273" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="268" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="274" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" s="268" t="n">
-        <v>40.7476</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="296" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="274" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="268" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="275" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" s="268" t="n">
-        <v>54.134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="297" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="275" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="268" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="276" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9" s="268" t="n">
-        <v>26.14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="298" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="276" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="268" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="277" t="s">
-        <v>149</v>
-      </c>
-      <c r="C10" s="268" t="n">
-        <v>10.7489</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" s="299" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="277" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="268" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="278" t="s">
-        <v>150</v>
-      </c>
-      <c r="C11" s="268" t="n">
-        <v>32.2205</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="300" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="278" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="268" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="279" t="s">
-        <v>151</v>
-      </c>
-      <c r="C12" s="268" t="n">
-        <v>10.5183</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" s="301" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="279" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="268" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="280" t="s">
-        <v>152</v>
-      </c>
-      <c r="C13" s="268" t="n">
-        <v>9.42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="302" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="280" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="268" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="281" t="s">
-        <v>153</v>
-      </c>
-      <c r="C14" s="268" t="n">
-        <v>78.0468</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" s="303" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="281" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="268" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="282" t="s">
-        <v>154</v>
-      </c>
-      <c r="C15" s="268" t="n">
-        <v>10.75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="304" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="282" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="268" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="283" t="s">
-        <v>155</v>
-      </c>
-      <c r="C16" s="268" t="n">
-        <v>10.945</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="305" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="283" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="268" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="284" t="s">
-        <v>156</v>
-      </c>
-      <c r="C17" s="268" t="n">
-        <v>52.7536</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="306" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" s="284" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="268" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="285" t="s">
-        <v>156</v>
-      </c>
-      <c r="C18" s="268" t="n">
-        <v>10.38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="307" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="285" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="268" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="286" t="s">
-        <v>157</v>
-      </c>
-      <c r="C19" s="268" t="n">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="308" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="286" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="268" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="287" t="s">
-        <v>158</v>
-      </c>
-      <c r="C20" s="268" t="n">
-        <v>45.3514</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="309" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="287" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="268" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="288" t="s">
-        <v>159</v>
-      </c>
-      <c r="C21" s="268" t="n">
-        <v>10.25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="310" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="288" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="268" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="289" t="s">
-        <v>160</v>
-      </c>
-      <c r="C22" s="268" t="n">
-        <v>41.3028</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="311" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" s="289" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="268" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="290" t="s">
-        <v>161</v>
-      </c>
-      <c r="C23" s="268" t="n">
-        <v>14.44</v>
+      <c r="B23" s="312" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="290" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IndMF- Updated sheet name as NAV for small cap
</commit_message>
<xml_diff>
--- a/Reports/IndMFData/IndMF_SmallCap.xlsx
+++ b/Reports/IndMFData/IndMF_SmallCap.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i852841/_Codes/_Personal/StockRankingCrawler/Reports/IndMFData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BD4573-9AEC-8243-9C40-D4EE0E198C73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8767F497-3CD5-054D-A34D-3719FA38DD5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SmallCap" sheetId="1" r:id="rId1"/>
+    <sheet name="NAV" sheetId="1" r:id="rId1"/>
     <sheet name="UNDERLYINGINDEX" sheetId="2" r:id="rId2"/>
     <sheet name="AUM" sheetId="3" r:id="rId3"/>
     <sheet name="EXPENSERATIO" sheetId="4" r:id="rId4"/>
@@ -1285,15 +1285,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="8.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="7.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.1640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -3287,11 +3288,12 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.83203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>

</xml_diff>

<commit_message>
IndMF- Added Other attribute data for mid cap
</commit_message>
<xml_diff>
--- a/Reports/IndMFData/IndMF_SmallCap.xlsx
+++ b/Reports/IndMFData/IndMF_SmallCap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i852841/_Codes/_Personal/StockRankingCrawler/Reports/IndMFData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8767F497-3CD5-054D-A34D-3719FA38DD5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316D2F0D-0A0C-7D47-BBD7-C585BE2D4DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAV" sheetId="1" r:id="rId1"/>
@@ -1285,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3287,13 +3287,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E466B42B-1FD8-C746-8F67-0DBD703B7828}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="43.83203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>

</xml_diff>